<commit_message>
cap nhat quan pn pn
</commit_message>
<xml_diff>
--- a/data/thietbitichhop.xlsx
+++ b/data/thietbitichhop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cscctphcm-my.sharepoint.com/personal/gdcsbac_cscctphcm_onmicrosoft_com/Documents/Web ban do thu nghiem/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cscctphcm-my.sharepoint.com/personal/gdcsbac_cscctphcm_onmicrosoft_com/Documents/webdemo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{2EDB2D67-B674-4A3F-BBBF-6356067A4A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0109586D-C26A-4F55-AE3E-F1F7AE8FF1CF}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{2EDB2D67-B674-4A3F-BBBF-6356067A4A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7705A5F-8EDF-4F85-ACE8-6212C67AC3E1}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="36" windowWidth="22488" windowHeight="12924" xr2:uid="{A1266DFF-32F5-4B0B-A729-2A44814C55C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A1266DFF-32F5-4B0B-A729-2A44814C55C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Camera" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="35">
   <si>
     <t>latitude</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>STT</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -706,7 +712,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -723,7 +729,7 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -732,6 +738,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="60">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -795,8 +806,71 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -813,6 +887,20 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
         <right/>
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -837,16 +925,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -891,16 +969,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -943,56 +1011,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1003,6 +1021,22 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1018,13 +1052,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22F76FA4-6F68-4C4C-ACF7-AD980D4B7B85}" name="Table1" displayName="Table1" ref="A1:L8" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A1:L8" xr:uid="{22F76FA4-6F68-4C4C-ACF7-AD980D4B7B85}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{97C2907B-52CA-4841-9D78-B2B9F62401ED}" name="STT" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{77542F9E-774E-47B9-8FA0-1F4235E71B6F}" name="latitude" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{D7B47058-2692-41B7-817E-A553B38241AC}" name="longtitude" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{124512DE-AD9E-46D0-BA14-B30E98189184}" name="name" dataDxfId="22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22F76FA4-6F68-4C4C-ACF7-AD980D4B7B85}" name="Table1" displayName="Table1" ref="A1:N8" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A1:N8" xr:uid="{22F76FA4-6F68-4C4C-ACF7-AD980D4B7B85}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{97C2907B-52CA-4841-9D78-B2B9F62401ED}" name="STT" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{124512DE-AD9E-46D0-BA14-B30E98189184}" name="name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{77542F9E-774E-47B9-8FA0-1F4235E71B6F}" name="latitude" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{D7B47058-2692-41B7-817E-A553B38241AC}" name="longtitude" dataDxfId="22"/>
+    <tableColumn id="13" xr3:uid="{D2E18239-7018-449F-AC29-2D042C641CF7}" name="N" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{92F6385C-46EB-4672-BFC1-D8C327655443}" name="E" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{4D8F4D8C-6F7F-4AB9-88EB-F0395A057331}" name="so tru"/>
     <tableColumn id="6" xr3:uid="{37A743F1-67E3-4FFF-877A-8BEEA75A7C5A}" name="ten tu"/>
     <tableColumn id="7" xr3:uid="{9D926483-63E2-4E90-BB45-E1DDFD0EDFD2}" name="tuyen duong"/>
@@ -1039,13 +1075,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E069F26D-ED8C-4920-897F-2713307302B9}" name="Table134" displayName="Table134" ref="A1:L8" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E069F26D-ED8C-4920-897F-2713307302B9}" name="Table134" displayName="Table134" ref="A1:L8" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="A1:L8" xr:uid="{22F76FA4-6F68-4C4C-ACF7-AD980D4B7B85}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A995F358-D75F-43DE-B09C-175E39B13DE7}" name="STT" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{EC202400-F540-4706-BB40-67FB699F7007}" name="latitude" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{BCEE706D-9A91-4670-81ED-1DB85E7AA8AD}" name="longtitude" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{61CE6549-4006-44CE-882E-7BF7EC787CCB}" name="name" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{A995F358-D75F-43DE-B09C-175E39B13DE7}" name="STT" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{EC202400-F540-4706-BB40-67FB699F7007}" name="latitude" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{BCEE706D-9A91-4670-81ED-1DB85E7AA8AD}" name="longtitude" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{61CE6549-4006-44CE-882E-7BF7EC787CCB}" name="name" dataDxfId="17"/>
     <tableColumn id="5" xr3:uid="{7349A58E-F001-4AB2-BC85-FA8FF883EE8C}" name="so tru"/>
     <tableColumn id="6" xr3:uid="{E037A3FB-6DE5-405A-8D3F-9B34E2D847D6}" name="ten tu"/>
     <tableColumn id="7" xr3:uid="{D8AEE77D-DE43-434D-8C7E-B33C1E7C8595}" name="tuyen duong"/>
@@ -1060,13 +1096,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3301A464-DCB0-4423-8051-2AD3C5D0F1A6}" name="Table1345" displayName="Table1345" ref="A1:L8" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3301A464-DCB0-4423-8051-2AD3C5D0F1A6}" name="Table1345" displayName="Table1345" ref="A1:L8" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A1:L8" xr:uid="{22F76FA4-6F68-4C4C-ACF7-AD980D4B7B85}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{0685D0F4-4045-4128-971F-82C5EA5C7073}" name="STT" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{F4A46EF0-4F3F-4F47-B688-46A53DBFF199}" name="latitude" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{80C4B6B4-B238-4E16-BF33-55C8115C7EE9}" name="longtitude" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{579A0FDA-E832-4C03-9A44-09D053C12362}" name="name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0685D0F4-4045-4128-971F-82C5EA5C7073}" name="STT" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{F4A46EF0-4F3F-4F47-B688-46A53DBFF199}" name="latitude" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{80C4B6B4-B238-4E16-BF33-55C8115C7EE9}" name="longtitude" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{579A0FDA-E832-4C03-9A44-09D053C12362}" name="name" dataDxfId="12"/>
     <tableColumn id="5" xr3:uid="{ADC46274-C195-4EAC-862A-71C401464DA9}" name="so tru"/>
     <tableColumn id="6" xr3:uid="{2B03131C-A9C2-43ED-A87D-12EEBDF8E684}" name="ten tu"/>
     <tableColumn id="7" xr3:uid="{7DDBE528-3751-4DBE-8E8D-3B0FA90A43CA}" name="tuyen duong"/>
@@ -1081,13 +1117,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51304910-A8C6-4E66-A41C-4CCFE6D894E1}" name="Table13" displayName="Table13" ref="A1:L8" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{51304910-A8C6-4E66-A41C-4CCFE6D894E1}" name="Table13" displayName="Table13" ref="A1:L8" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:L8" xr:uid="{22F76FA4-6F68-4C4C-ACF7-AD980D4B7B85}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{DE65939C-4CCD-40CE-BCBC-D285554F6933}" name="STT" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{70CFD072-611C-4A93-B112-3CFF68D32484}" name="latitude" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{EB94A91B-FD12-4424-AA1F-451FCB75A797}" name="longtitude" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{93B52AC0-5214-4C3D-823D-DF79152D8331}" name="name" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{DE65939C-4CCD-40CE-BCBC-D285554F6933}" name="STT" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{70CFD072-611C-4A93-B112-3CFF68D32484}" name="latitude" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{EB94A91B-FD12-4424-AA1F-451FCB75A797}" name="longtitude" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{93B52AC0-5214-4C3D-823D-DF79152D8331}" name="name" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{F2B6A588-13E0-4E31-9ED4-64CE0306C244}" name="so tru"/>
     <tableColumn id="6" xr3:uid="{AD570874-5F35-49BF-8366-BA86676CC717}" name="ten tu"/>
     <tableColumn id="7" xr3:uid="{45E0C1BA-C1A6-4FE8-B25F-04B5D87BB53C}" name="tuyen duong"/>
@@ -1418,163 +1454,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86673E56-9A8C-4B3E-BC42-A6E3991962E7}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.59765625" customWidth="1"/>
-    <col min="9" max="9" width="12.19921875" customWidth="1"/>
-    <col min="10" max="10" width="17.796875" customWidth="1"/>
-    <col min="11" max="11" width="14.8984375" customWidth="1"/>
-    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.59765625" customWidth="1"/>
+    <col min="12" max="12" width="12.19921875" customWidth="1"/>
+    <col min="13" max="13" width="17.796875" customWidth="1"/>
+    <col min="14" max="14" width="14.8984375" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D8">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="10.726672868">
+  <conditionalFormatting sqref="B2:F8">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="10.726672868">
       <formula>NOT(ISERROR(SEARCH("10.726672868",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1744,7 +1802,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D8">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="10.726672868">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="10.726672868">
       <formula>NOT(ISERROR(SEARCH("10.726672868",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1914,7 +1972,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D8">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="10.726672868">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="10.726672868">
       <formula>NOT(ISERROR(SEARCH("10.726672868",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2084,7 +2142,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D8">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="10.726672868">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="10.726672868">
       <formula>NOT(ISERROR(SEARCH("10.726672868",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>